<commit_message>
Character info button and menu, saving and loading data test
</commit_message>
<xml_diff>
--- a/AZGame/Assets/Docs/AZGameDoc.xlsx
+++ b/AZGame/Assets/Docs/AZGameDoc.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sayat\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProjectsGit\AZGame\AZGame\Assets\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="44">
   <si>
     <t>GDE_FIELD_NAMES</t>
   </si>
@@ -34,91 +34,130 @@
     <t>GDE_FIELD_TYPES</t>
   </si>
   <si>
+    <t>CharacterName</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>DifficultyLevel</t>
+  </si>
+  <si>
+    <t>BasicMelee</t>
+  </si>
+  <si>
+    <t>BasicDistance</t>
+  </si>
+  <si>
+    <t>BasicMagic</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>CharacterDescription</t>
+  </si>
+  <si>
+    <t>low/medium</t>
+  </si>
+  <si>
+    <t>simple history of character</t>
+  </si>
+  <si>
+    <t>up to five / six characters</t>
+  </si>
+  <si>
+    <t>MonsterName</t>
+  </si>
+  <si>
+    <t>MonsterDescription</t>
+  </si>
+  <si>
+    <t>optional monster description</t>
+  </si>
+  <si>
+    <t>at least 20</t>
+  </si>
+  <si>
+    <t>MissionName</t>
+  </si>
+  <si>
+    <t>MissionDescription</t>
+  </si>
+  <si>
+    <t>few words</t>
+  </si>
+  <si>
+    <t>MeleeReward</t>
+  </si>
+  <si>
+    <t>DistanceReward</t>
+  </si>
+  <si>
+    <t>MagicReward</t>
+  </si>
+  <si>
+    <t>rough idea</t>
+  </si>
+  <si>
+    <t>depend on diff level</t>
+  </si>
+  <si>
+    <t>MonsterType</t>
+  </si>
+  <si>
+    <t>Melee/Distance/Magic</t>
+  </si>
+  <si>
+    <t>MissionLevel</t>
+  </si>
+  <si>
+    <t>easy/medium/hard</t>
+  </si>
+  <si>
+    <t>FirstChoose</t>
+  </si>
+  <si>
+    <t>SecondChoose</t>
+  </si>
+  <si>
+    <t>ThirdChoose</t>
+  </si>
+  <si>
+    <t>ForthChoose</t>
+  </si>
+  <si>
+    <t>FirstNext</t>
+  </si>
+  <si>
+    <t>SecondNext</t>
+  </si>
+  <si>
+    <t>ThirdNext</t>
+  </si>
+  <si>
+    <t>ForthNext</t>
+  </si>
+  <si>
+    <t>nextCardKey</t>
+  </si>
+  <si>
+    <t>CH001</t>
+  </si>
+  <si>
+    <t>CH000</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>sdahjsakhdask hsajkdhsajk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low </t>
+  </si>
+  <si>
     <t>GDE_IGNORE</t>
-  </si>
-  <si>
-    <t>CharacterName</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>DifficultyLevel</t>
-  </si>
-  <si>
-    <t>BasicMelee</t>
-  </si>
-  <si>
-    <t>BasicDistance</t>
-  </si>
-  <si>
-    <t>BasicMagic</t>
-  </si>
-  <si>
-    <t>float</t>
-  </si>
-  <si>
-    <t>CharacterDescription</t>
-  </si>
-  <si>
-    <t>low/medium</t>
-  </si>
-  <si>
-    <t>simple history of character</t>
-  </si>
-  <si>
-    <t>simply to use field key</t>
-  </si>
-  <si>
-    <t>up to five / six characters</t>
-  </si>
-  <si>
-    <t>MonsterName</t>
-  </si>
-  <si>
-    <t>MonsterDescription</t>
-  </si>
-  <si>
-    <t>optional monster description</t>
-  </si>
-  <si>
-    <t>at least 20</t>
-  </si>
-  <si>
-    <t>MissionName</t>
-  </si>
-  <si>
-    <t>MissionDescription</t>
-  </si>
-  <si>
-    <t>few words</t>
-  </si>
-  <si>
-    <t>MeleeReward</t>
-  </si>
-  <si>
-    <t>DistanceReward</t>
-  </si>
-  <si>
-    <t>MagicReward</t>
-  </si>
-  <si>
-    <t>rough idea</t>
-  </si>
-  <si>
-    <t>depend on diff level</t>
-  </si>
-  <si>
-    <t>MonsterType</t>
-  </si>
-  <si>
-    <t>Melee/Distance/Magic</t>
-  </si>
-  <si>
-    <t>MissionLevel</t>
-  </si>
-  <si>
-    <t>easy/medium/hard</t>
   </si>
 </sst>
 </file>
@@ -489,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,9 +545,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>2</v>
-      </c>
+      <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -529,15 +566,17 @@
       <c r="S1" s="6"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
@@ -547,9 +586,6 @@
       </c>
       <c r="G2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -564,27 +600,26 @@
       <c r="S2" s="2"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>4</v>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -600,23 +635,20 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>11</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
@@ -630,10 +662,32 @@
       <c r="S4" s="6"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
@@ -694,7 +748,7 @@
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,9 +765,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>2</v>
-      </c>
+      <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -735,18 +787,20 @@
       <c r="T1" s="6"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>5</v>
@@ -756,9 +810,6 @@
       </c>
       <c r="H2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -773,30 +824,29 @@
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="C3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -812,31 +862,28 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
@@ -911,10 +958,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T22"/>
+  <dimension ref="A1:AF22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,16 +969,14 @@
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="7" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="18" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" customWidth="1"/>
+    <col min="15" max="16" width="14.28515625" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>2</v>
-      </c>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -951,124 +996,203 @@
       <c r="R1" s="6"/>
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="2" t="s">
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="3" t="s">
+      <c r="J2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>4</v>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
+      <c r="L4" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
+      <c r="N4" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
+      <c r="P4" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1089,8 +1213,16 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1111,8 +1243,16 @@
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1133,8 +1273,16 @@
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1155,8 +1303,16 @@
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="4"/>
+      <c r="AB8" s="4"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1177,8 +1333,16 @@
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="4"/>
+      <c r="AB9" s="4"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1199,8 +1363,16 @@
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="4"/>
+      <c r="AB10" s="4"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1221,8 +1393,16 @@
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="4"/>
+      <c r="AB11" s="4"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1243,8 +1423,16 @@
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1265,8 +1453,16 @@
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="4"/>
+      <c r="AB13" s="4"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1287,8 +1483,16 @@
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
+      <c r="AA14" s="4"/>
+      <c r="AB14" s="4"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1309,8 +1513,16 @@
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="4"/>
+      <c r="AA15" s="4"/>
+      <c r="AB15" s="4"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1331,8 +1543,16 @@
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
       <c r="T16" s="4"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4"/>
+      <c r="AA16" s="4"/>
+      <c r="AB16" s="4"/>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1353,8 +1573,16 @@
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="4"/>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1375,8 +1603,16 @@
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="4"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1397,8 +1633,16 @@
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
       <c r="T19" s="4"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="4"/>
+      <c r="AB19" s="4"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1419,8 +1663,16 @@
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
       <c r="T20" s="4"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
+      <c r="Y20" s="4"/>
+      <c r="Z20" s="4"/>
+      <c r="AA20" s="4"/>
+      <c r="AB20" s="4"/>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1441,8 +1693,16 @@
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
       <c r="T21" s="4"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="4"/>
+      <c r="AB21" s="4"/>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1463,6 +1723,14 @@
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
       <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
+      <c r="Y22" s="4"/>
+      <c r="Z22" s="4"/>
+      <c r="AA22" s="4"/>
+      <c r="AB22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Get new mission fix
</commit_message>
<xml_diff>
--- a/AZGame/Assets/Docs/AZGameDoc.xlsx
+++ b/AZGame/Assets/Docs/AZGameDoc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProjectsGit\AZGame\AZGame\Assets\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProjects\AZGame\AZGame\Assets\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="107">
   <si>
     <t>GDE_FIELD_NAMES</t>
   </si>
@@ -100,33 +100,6 @@
     <t>easy/medium/hard</t>
   </si>
   <si>
-    <t>FirstChoose</t>
-  </si>
-  <si>
-    <t>SecondChoose</t>
-  </si>
-  <si>
-    <t>ThirdChoose</t>
-  </si>
-  <si>
-    <t>ForthChoose</t>
-  </si>
-  <si>
-    <t>FirstNext</t>
-  </si>
-  <si>
-    <t>SecondNext</t>
-  </si>
-  <si>
-    <t>ThirdNext</t>
-  </si>
-  <si>
-    <t>ForthNext</t>
-  </si>
-  <si>
-    <t>nextCardKey</t>
-  </si>
-  <si>
     <t>CH001</t>
   </si>
   <si>
@@ -331,24 +304,9 @@
     <t>1st mission</t>
   </si>
   <si>
-    <t>mission shows how game work</t>
-  </si>
-  <si>
     <t>easy</t>
   </si>
   <si>
-    <t>M0011</t>
-  </si>
-  <si>
-    <t>M0012</t>
-  </si>
-  <si>
-    <t>M0013</t>
-  </si>
-  <si>
-    <t>M0014</t>
-  </si>
-  <si>
     <t>false</t>
   </si>
   <si>
@@ -362,6 +320,33 @@
   </si>
   <si>
     <t>bool</t>
+  </si>
+  <si>
+    <t>M001A</t>
+  </si>
+  <si>
+    <t>M001B</t>
+  </si>
+  <si>
+    <t>M001C</t>
+  </si>
+  <si>
+    <t>Example mission description</t>
+  </si>
+  <si>
+    <t>NextCard</t>
+  </si>
+  <si>
+    <t>next card key</t>
+  </si>
+  <si>
+    <t>GoodPoints</t>
+  </si>
+  <si>
+    <t>EvilPoints</t>
+  </si>
+  <si>
+    <t>int</t>
   </si>
 </sst>
 </file>
@@ -750,7 +735,7 @@
   <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,13 +788,13 @@
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>5</v>
@@ -879,7 +864,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>12</v>
@@ -911,16 +896,16 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="C5" s="4" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E5" s="4">
         <v>100</v>
@@ -943,16 +928,16 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E6" s="4">
         <v>100</v>
@@ -975,16 +960,16 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E7" s="4">
         <v>100</v>
@@ -1007,16 +992,16 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E8" s="4">
         <v>100</v>
@@ -1039,16 +1024,16 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E9" s="4">
         <v>100</v>
@@ -1139,16 +1124,16 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1210,13 +1195,13 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>15</v>
@@ -1251,16 +1236,16 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="G5" s="4">
         <v>1</v>
@@ -1274,232 +1259,232 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="E14" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1510,10 +1495,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD22"/>
+  <dimension ref="A1:AC21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1521,13 +1506,13 @@
     <col min="1" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="14" width="14.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="18" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="12" max="13" width="14.28515625" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1553,14 +1538,13 @@
       <c r="W1" s="6"/>
       <c r="X1" s="6"/>
       <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>17</v>
@@ -1572,36 +1556,24 @@
         <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>4</v>
+        <v>102</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>31</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
+      <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
@@ -1612,14 +1584,13 @@
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>3</v>
@@ -1634,29 +1605,17 @@
         <v>3</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>3</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
@@ -1671,14 +1630,13 @@
       <c r="AA3" s="3"/>
       <c r="AB3" s="3"/>
       <c r="AC3" s="3"/>
-      <c r="AD3" s="3"/>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>16</v>
@@ -1690,24 +1648,16 @@
         <v>23</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="G4" s="6"/>
-      <c r="H4" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="H4" s="6"/>
       <c r="I4" s="6"/>
-      <c r="J4" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="J4" s="6"/>
       <c r="K4" s="6"/>
-      <c r="L4" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="L4" s="6"/>
       <c r="M4" s="6"/>
-      <c r="N4" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="O4" s="6"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
@@ -1722,26 +1672,25 @@
       <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
-      <c r="AD4" s="6"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>101</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -1762,19 +1711,20 @@
       <c r="W5" s="4"/>
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
-      <c r="Z5" s="4"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -1794,19 +1744,20 @@
       <c r="W6" s="4"/>
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -1826,14 +1777,13 @@
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
-      <c r="Z7" s="4"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -1858,18 +1808,23 @@
       <c r="W8" s="4"/>
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
-      <c r="Z8" s="4"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -1890,27 +1845,14 @@
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
-      <c r="Z9" s="4"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>40</v>
-      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -1930,9 +1872,8 @@
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
-      <c r="Z10" s="4"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1958,9 +1899,8 @@
       <c r="W11" s="4"/>
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
-      <c r="Z11" s="4"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1986,9 +1926,8 @@
       <c r="W12" s="4"/>
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
-      <c r="Z12" s="4"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2014,9 +1953,8 @@
       <c r="W13" s="4"/>
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
-      <c r="Z13" s="4"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2042,9 +1980,8 @@
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
       <c r="Y14" s="4"/>
-      <c r="Z14" s="4"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -2070,9 +2007,8 @@
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -2098,9 +2034,8 @@
       <c r="W16" s="4"/>
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -2126,9 +2061,8 @@
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -2154,9 +2088,8 @@
       <c r="W18" s="4"/>
       <c r="X18" s="4"/>
       <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -2182,9 +2115,8 @@
       <c r="W19" s="4"/>
       <c r="X19" s="4"/>
       <c r="Y19" s="4"/>
-      <c r="Z19" s="4"/>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -2210,9 +2142,8 @@
       <c r="W20" s="4"/>
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
-      <c r="Z20" s="4"/>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -2238,35 +2169,6 @@
       <c r="W21" s="4"/>
       <c r="X21" s="4"/>
       <c r="Y21" s="4"/>
-      <c r="Z21" s="4"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
-      <c r="W22" s="4"/>
-      <c r="X22" s="4"/>
-      <c r="Y22" s="4"/>
-      <c r="Z22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>